<commit_message>
Location display finally functional
</commit_message>
<xml_diff>
--- a/TestCircuits/MCCoData.xlsx
+++ b/TestCircuits/MCCoData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="700" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Substation" sheetId="1" r:id="rId1"/>
@@ -4629,7 +4629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -6431,8 +6431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G245"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6711,7 +6711,7 @@
         <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>187</v>
+        <v>57</v>
       </c>
       <c r="F12">
         <v>7</v>

</xml_diff>